<commit_message>
More data and more coding clutter added
</commit_message>
<xml_diff>
--- a/Logbook_automated_by_python_testing_backup.xlsx
+++ b/Logbook_automated_by_python_testing_backup.xlsx
@@ -8,32 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0e67038fc02b579b/Documenten/GitHub/tidegas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C32668DC-7CC6-4CC8-B0CE-50FC9B9A4CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{46B66ABA-F133-4ECF-B39F-295C030EC6DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{96F930A0-3915-409C-9FA8-BC0285AB49FF}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="123">
   <si>
     <t>Description</t>
   </si>
@@ -53,7 +40,7 @@
     <t>batch</t>
   </si>
   <si>
-    <t>identifier</t>
+    <t>Corresponding DIC file nr</t>
   </si>
   <si>
     <t xml:space="preserve">notes </t>
@@ -95,6 +82,9 @@
     <t>acid increment extracted</t>
   </si>
   <si>
+    <t>acid added (mL)</t>
+  </si>
+  <si>
     <t>acid increments (mL)</t>
   </si>
   <si>
@@ -125,9 +115,30 @@
     <t>Integrated current  (uAs)</t>
   </si>
   <si>
+    <t>raw DIC umol/L</t>
+  </si>
+  <si>
+    <t>Calculated DIC umol/kg</t>
+  </si>
+  <si>
     <t>Faradays constant</t>
   </si>
   <si>
+    <t>Unnamed: 34</t>
+  </si>
+  <si>
+    <t>Unnamed: 35</t>
+  </si>
+  <si>
+    <t>Unnamed: 36</t>
+  </si>
+  <si>
+    <t>Unnamed: 37</t>
+  </si>
+  <si>
+    <t>Unnamed: 38</t>
+  </si>
+  <si>
     <t>0-0  0  (0)junk-250916-01.dat</t>
   </si>
   <si>
@@ -143,132 +154,132 @@
     <t>not_good</t>
   </si>
   <si>
+    <t>0-0  0  (0)junk-250916-02.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-250916-03.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-250916-04.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-250916-05.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-250916-06.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-250916-07.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-250916-08.dat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cell not full </t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-250916-09.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-250916-10.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-250916-11.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-250917-01.dat</t>
+  </si>
+  <si>
+    <t>17-Sep</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-250917-02.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-250917-03.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-250917-04.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-250917-05.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-250917-06.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-250917-07.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-250917-08.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-250917-09.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-250917-10.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-250917-11.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-250917-12.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-250918-01.dat</t>
+  </si>
+  <si>
+    <t>18-Sep</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-250918-02.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-250918-03.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-250930-02.dat</t>
+  </si>
+  <si>
+    <t>30-Sep</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-250930-03.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-250930-04-2_25mL-0_15incrMl.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-250930-05-1_2mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-250930-06-3_15mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-250930-07-3_60mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-250930-08-4_80mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-250930-09-4_2mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-251001-01-4_2mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>01-Oct</t>
+  </si>
+  <si>
     <t>yes</t>
   </si>
   <si>
-    <t>0-0  0  (0)junk-250916-02.dat</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)junk-250916-03.dat</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)junk-250916-04.dat</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)junk-250916-05.dat</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)junk-250916-06.dat</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)junk-250916-07.dat</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)junk-250916-08.dat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cell not full </t>
-  </si>
-  <si>
-    <t>0-0  0  (0)junk-250916-09.dat</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)junk-250916-10.dat</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)junk-250916-11.dat</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)junk-250917-01.dat</t>
-  </si>
-  <si>
-    <t>17-Sep</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)junk-250917-02.dat</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)junk-250917-03.dat</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)junk-250917-04.dat</t>
+    <t>0-0  0  (0)junk-251001-02-2_25mL-0_15incrmL.dat</t>
   </si>
   <si>
     <t>Reference</t>
   </si>
   <si>
-    <t>0-0  0  (0)junk-250917-05.dat</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)junk-250917-06.dat</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)junk-250917-07.dat</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)junk-250917-08.dat</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)junk-250917-09.dat</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)junk-250917-10.dat</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)junk-250917-11.dat</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)junk-250917-12.dat</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)junk-250918-01.dat</t>
-  </si>
-  <si>
-    <t>18-Sep</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)junk-250918-02.dat</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)junk-250918-03.dat</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)junk-250930-02.dat</t>
-  </si>
-  <si>
-    <t>30-Sep</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)junk-250930-03.dat</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)junk-250930-04-2_25mL-0_15incrMl.dat</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)junk-250930-05-1_2mL-0_15incrmL.dat</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)junk-250930-06-3_15mL-0_15incrmL.dat</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)junk-250930-07-3_60mL-0_15incrmL.dat</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)junk-250930-08-4_80mL-0_15incrmL.dat</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)junk-250930-09-4_2mL-0_15incrmL.dat</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)junk-251001-01-4_2mL-0_15incrmL.dat</t>
-  </si>
-  <si>
-    <t>01-Oct</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)junk-251001-02-2_25mL-0_15incrmL.dat</t>
-  </si>
-  <si>
     <t>0-0  0  (0)junk-251001-03-1_2mL-0_15incrmL.dat</t>
   </si>
   <si>
@@ -299,13 +310,85 @@
     <t>0-0  0  (0)junk-251001-13-4_2mL-0_15incrmL.dat</t>
   </si>
   <si>
-    <t>acid added (mL)</t>
-  </si>
-  <si>
-    <t>raw DIC umol/L</t>
-  </si>
-  <si>
-    <t>Calculated DIC umol/kg</t>
+    <t>0-0  0  (0)junk-251003-01-4_2mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>03-Oct</t>
+  </si>
+  <si>
+    <t>change this!</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-251003-02-4_2mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-251003-03-4_2mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-251003-04-4_2mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-251003-05-4_2mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-251003-07-2_25mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-251003-08-2_25mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-251003-09-2_25mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-251006-01-4_2mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>06-Oct</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-251006-02-4_2mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-251006-03-4_2mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-251006-04-4_2mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-251006-05-4_2mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-251006-06-4_2mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-251006-07-4_2mL-0_15incrmL-0_0min.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-251006-08-4_2mL-0_15incrmL-1_0min.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-251008-01-4_2mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>08-Oct</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-251008-02-4_2mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-251008-03-4_2mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-251008-04-4_2mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-251008-05-4_2mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-251008-06-4_2mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-251008-07-4_2mL-0_15incrmL.dat</t>
   </si>
 </sst>
 </file>
@@ -324,7 +407,6 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -382,10 +464,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -673,20 +751,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BH47"/>
+  <dimension ref="A1:AM70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA1" sqref="AA1"/>
+    <sheetView tabSelected="1" topLeftCell="Q36" workbookViewId="0">
+      <selection activeCell="Z11" sqref="Z11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="8" max="8" width="21.77734375" customWidth="1"/>
-    <col min="30" max="30" width="28.77734375" customWidth="1"/>
-    <col min="32" max="32" width="10" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -748,92 +821,81 @@
         <v>19</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>88</v>
+        <v>20</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>89</v>
+        <v>31</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>90</v>
+        <v>32</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AI1" s="1"/>
-      <c r="AJ1" s="1"/>
-      <c r="AK1" s="1"/>
-      <c r="AL1" s="1"/>
-      <c r="AM1" s="1"/>
-      <c r="AN1" s="1"/>
-      <c r="AO1" s="1"/>
-      <c r="AP1" s="1"/>
-      <c r="AQ1" s="1"/>
-      <c r="AR1" s="1"/>
-      <c r="AS1" s="1"/>
-      <c r="AT1" s="1"/>
-      <c r="AU1" s="1"/>
-      <c r="AV1" s="1"/>
-      <c r="AW1" s="1"/>
-      <c r="AX1" s="1"/>
-      <c r="AY1" s="1"/>
-      <c r="AZ1" s="1"/>
-      <c r="BA1" s="1"/>
-      <c r="BB1" s="1"/>
-      <c r="BC1" s="1"/>
-      <c r="BD1" s="1"/>
-      <c r="BE1" s="1"/>
-      <c r="BF1" s="1"/>
-      <c r="BG1" s="1"/>
-      <c r="BH1" s="1"/>
-    </row>
-    <row r="2" spans="1:60" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:39" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="I2" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="J2">
         <v>21.3</v>
@@ -850,6 +912,12 @@
       <c r="N2">
         <v>2300</v>
       </c>
+      <c r="S2">
+        <v>4.2</v>
+      </c>
+      <c r="T2">
+        <v>0.15</v>
+      </c>
       <c r="U2">
         <v>4.2</v>
       </c>
@@ -860,15 +928,15 @@
         <v>96485.332123</v>
       </c>
     </row>
-    <row r="3" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -888,6 +956,12 @@
       <c r="N3">
         <v>2300</v>
       </c>
+      <c r="S3">
+        <v>4.2</v>
+      </c>
+      <c r="T3">
+        <v>0.15</v>
+      </c>
       <c r="U3">
         <v>4.2</v>
       </c>
@@ -907,15 +981,15 @@
         <v>96485.332123</v>
       </c>
     </row>
-    <row r="4" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -935,6 +1009,12 @@
       <c r="N4">
         <v>2300</v>
       </c>
+      <c r="S4">
+        <v>4.2</v>
+      </c>
+      <c r="T4">
+        <v>0.15</v>
+      </c>
       <c r="U4">
         <v>4.2</v>
       </c>
@@ -954,15 +1034,15 @@
         <v>96485.332123</v>
       </c>
     </row>
-    <row r="5" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -982,6 +1062,12 @@
       <c r="N5">
         <v>2300</v>
       </c>
+      <c r="S5">
+        <v>4.2</v>
+      </c>
+      <c r="T5">
+        <v>0.15</v>
+      </c>
       <c r="U5">
         <v>4.2</v>
       </c>
@@ -1001,15 +1087,15 @@
         <v>96485.332123</v>
       </c>
     </row>
-    <row r="6" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" t="s">
         <v>40</v>
       </c>
-      <c r="C6" t="s">
-        <v>32</v>
-      </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E6">
         <v>5</v>
@@ -1029,6 +1115,12 @@
       <c r="N6">
         <v>2300</v>
       </c>
+      <c r="S6">
+        <v>4.2</v>
+      </c>
+      <c r="T6">
+        <v>0.15</v>
+      </c>
       <c r="U6">
         <v>4.2</v>
       </c>
@@ -1048,15 +1140,15 @@
         <v>96485.332123</v>
       </c>
     </row>
-    <row r="7" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E7">
         <v>6</v>
@@ -1076,6 +1168,12 @@
       <c r="N7">
         <v>2300</v>
       </c>
+      <c r="S7">
+        <v>4.2</v>
+      </c>
+      <c r="T7">
+        <v>0.15</v>
+      </c>
       <c r="U7">
         <v>4.2</v>
       </c>
@@ -1095,15 +1193,15 @@
         <v>96485.332123</v>
       </c>
     </row>
-    <row r="8" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E8">
         <v>7</v>
@@ -1123,6 +1221,12 @@
       <c r="N8">
         <v>2300</v>
       </c>
+      <c r="S8">
+        <v>4.2</v>
+      </c>
+      <c r="T8">
+        <v>0.15</v>
+      </c>
       <c r="U8">
         <v>4.2</v>
       </c>
@@ -1142,24 +1246,24 @@
         <v>96485.332123</v>
       </c>
     </row>
-    <row r="9" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E9">
         <v>8</v>
       </c>
       <c r="H9" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="I9" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="J9">
         <v>25.9</v>
@@ -1176,6 +1280,12 @@
       <c r="N9">
         <v>2300</v>
       </c>
+      <c r="S9">
+        <v>4.2</v>
+      </c>
+      <c r="T9">
+        <v>0.15</v>
+      </c>
       <c r="U9">
         <v>4.2</v>
       </c>
@@ -1186,15 +1296,15 @@
         <v>96485.332123</v>
       </c>
     </row>
-    <row r="10" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E10">
         <v>9</v>
@@ -1214,6 +1324,12 @@
       <c r="N10">
         <v>2300</v>
       </c>
+      <c r="S10">
+        <v>4.2</v>
+      </c>
+      <c r="T10">
+        <v>0.15</v>
+      </c>
       <c r="U10">
         <v>4.2</v>
       </c>
@@ -1233,15 +1349,15 @@
         <v>96485.332123</v>
       </c>
     </row>
-    <row r="11" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E11">
         <v>10</v>
@@ -1261,6 +1377,12 @@
       <c r="N11">
         <v>2300</v>
       </c>
+      <c r="S11">
+        <v>4.2</v>
+      </c>
+      <c r="T11">
+        <v>0.15</v>
+      </c>
       <c r="U11">
         <v>4.2</v>
       </c>
@@ -1280,15 +1402,15 @@
         <v>96485.332123</v>
       </c>
     </row>
-    <row r="12" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E12">
         <v>11</v>
@@ -1308,6 +1430,12 @@
       <c r="N12">
         <v>2300</v>
       </c>
+      <c r="S12">
+        <v>4.2</v>
+      </c>
+      <c r="T12">
+        <v>0.15</v>
+      </c>
       <c r="U12">
         <v>4.2</v>
       </c>
@@ -1327,15 +1455,15 @@
         <v>96485.332123</v>
       </c>
     </row>
-    <row r="13" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D13" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -1355,6 +1483,12 @@
       <c r="N13">
         <v>2300</v>
       </c>
+      <c r="S13">
+        <v>4.2</v>
+      </c>
+      <c r="T13">
+        <v>0.15</v>
+      </c>
       <c r="U13">
         <v>4.2</v>
       </c>
@@ -1374,15 +1508,15 @@
         <v>96485.332123</v>
       </c>
     </row>
-    <row r="14" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D14" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E14">
         <v>2</v>
@@ -1402,6 +1536,12 @@
       <c r="N14">
         <v>2300</v>
       </c>
+      <c r="S14">
+        <v>4.2</v>
+      </c>
+      <c r="T14">
+        <v>0.15</v>
+      </c>
       <c r="U14">
         <v>4.2</v>
       </c>
@@ -1421,15 +1561,15 @@
         <v>96485.332123</v>
       </c>
     </row>
-    <row r="15" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C15" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D15" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E15">
         <v>3</v>
@@ -1449,6 +1589,12 @@
       <c r="N15">
         <v>2300</v>
       </c>
+      <c r="S15">
+        <v>4.2</v>
+      </c>
+      <c r="T15">
+        <v>0.15</v>
+      </c>
       <c r="U15">
         <v>4.2</v>
       </c>
@@ -1468,15 +1614,15 @@
         <v>96485.332123</v>
       </c>
     </row>
-    <row r="16" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:39" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="C16" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D16" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E16">
         <v>4</v>
@@ -1496,6 +1642,12 @@
       <c r="N16">
         <v>2300</v>
       </c>
+      <c r="S16">
+        <v>4.2</v>
+      </c>
+      <c r="T16">
+        <v>0.15</v>
+      </c>
       <c r="U16">
         <v>4.2</v>
       </c>
@@ -1517,13 +1669,13 @@
     </row>
     <row r="17" spans="2:34" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E17">
         <v>5</v>
@@ -1543,6 +1695,12 @@
       <c r="N17">
         <v>2300</v>
       </c>
+      <c r="S17">
+        <v>4.2</v>
+      </c>
+      <c r="T17">
+        <v>0.15</v>
+      </c>
       <c r="U17">
         <v>4.2</v>
       </c>
@@ -1564,13 +1722,13 @@
     </row>
     <row r="18" spans="2:34" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C18" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D18" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E18">
         <v>6</v>
@@ -1590,6 +1748,12 @@
       <c r="N18">
         <v>2300</v>
       </c>
+      <c r="S18">
+        <v>4.2</v>
+      </c>
+      <c r="T18">
+        <v>0.15</v>
+      </c>
       <c r="U18">
         <v>4.2</v>
       </c>
@@ -1611,13 +1775,13 @@
     </row>
     <row r="19" spans="2:34" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" t="s">
         <v>56</v>
       </c>
-      <c r="C19" t="s">
-        <v>49</v>
-      </c>
       <c r="D19" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E19">
         <v>7</v>
@@ -1637,6 +1801,12 @@
       <c r="N19">
         <v>2300</v>
       </c>
+      <c r="S19">
+        <v>4.2</v>
+      </c>
+      <c r="T19">
+        <v>0.15</v>
+      </c>
       <c r="U19">
         <v>4.2</v>
       </c>
@@ -1658,13 +1828,13 @@
     </row>
     <row r="20" spans="2:34" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C20" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D20" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E20">
         <v>8</v>
@@ -1684,6 +1854,12 @@
       <c r="N20">
         <v>2300</v>
       </c>
+      <c r="S20">
+        <v>4.2</v>
+      </c>
+      <c r="T20">
+        <v>0.15</v>
+      </c>
       <c r="U20">
         <v>4.2</v>
       </c>
@@ -1705,13 +1881,13 @@
     </row>
     <row r="21" spans="2:34" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C21" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D21" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E21">
         <v>9</v>
@@ -1731,6 +1907,12 @@
       <c r="N21">
         <v>2300</v>
       </c>
+      <c r="S21">
+        <v>4.2</v>
+      </c>
+      <c r="T21">
+        <v>0.15</v>
+      </c>
       <c r="U21">
         <v>4.2</v>
       </c>
@@ -1752,19 +1934,19 @@
     </row>
     <row r="22" spans="2:34" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="C22" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D22" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E22">
         <v>10</v>
       </c>
       <c r="I22" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="J22">
         <v>25.2</v>
@@ -1781,6 +1963,12 @@
       <c r="N22">
         <v>2300</v>
       </c>
+      <c r="S22">
+        <v>4.2</v>
+      </c>
+      <c r="T22">
+        <v>0.15</v>
+      </c>
       <c r="U22">
         <v>4.2</v>
       </c>
@@ -1802,13 +1990,13 @@
     </row>
     <row r="23" spans="2:34" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="C23" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D23" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E23">
         <v>11</v>
@@ -1828,6 +2016,12 @@
       <c r="N23">
         <v>2300</v>
       </c>
+      <c r="S23">
+        <v>4.2</v>
+      </c>
+      <c r="T23">
+        <v>0.15</v>
+      </c>
       <c r="U23">
         <v>4.2</v>
       </c>
@@ -1849,13 +2043,13 @@
     </row>
     <row r="24" spans="2:34" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C24" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D24" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E24">
         <v>12</v>
@@ -1875,6 +2069,12 @@
       <c r="N24">
         <v>2300</v>
       </c>
+      <c r="S24">
+        <v>4.2</v>
+      </c>
+      <c r="T24">
+        <v>0.15</v>
+      </c>
       <c r="U24">
         <v>4.2</v>
       </c>
@@ -1896,13 +2096,13 @@
     </row>
     <row r="25" spans="2:34" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C25" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D25" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -1922,6 +2122,9 @@
       <c r="N25">
         <v>2300</v>
       </c>
+      <c r="T25">
+        <v>0.15</v>
+      </c>
       <c r="V25">
         <v>0.15</v>
       </c>
@@ -1937,13 +2140,13 @@
     </row>
     <row r="26" spans="2:34" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C26" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D26" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E26">
         <v>2</v>
@@ -1963,6 +2166,9 @@
       <c r="N26">
         <v>2300</v>
       </c>
+      <c r="T26">
+        <v>0.15</v>
+      </c>
       <c r="V26">
         <v>0.15</v>
       </c>
@@ -1978,13 +2184,13 @@
     </row>
     <row r="27" spans="2:34" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C27" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D27" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E27">
         <v>3</v>
@@ -2004,6 +2210,9 @@
       <c r="N27">
         <v>2300</v>
       </c>
+      <c r="T27">
+        <v>0.15</v>
+      </c>
       <c r="V27">
         <v>0.15</v>
       </c>
@@ -2016,13 +2225,13 @@
     </row>
     <row r="28" spans="2:34" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C28" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="D28" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E28">
         <v>2</v>
@@ -2042,6 +2251,12 @@
       <c r="N28">
         <v>2300</v>
       </c>
+      <c r="S28">
+        <v>4.2</v>
+      </c>
+      <c r="T28">
+        <v>0.15</v>
+      </c>
       <c r="U28">
         <v>4.2</v>
       </c>
@@ -2057,13 +2272,13 @@
     </row>
     <row r="29" spans="2:34" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C29" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="D29" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E29">
         <v>3</v>
@@ -2083,6 +2298,12 @@
       <c r="N29">
         <v>2300</v>
       </c>
+      <c r="S29">
+        <v>4.2</v>
+      </c>
+      <c r="T29">
+        <v>0.15</v>
+      </c>
       <c r="U29">
         <v>4.2</v>
       </c>
@@ -2096,7 +2317,7 @@
         <v>2346.1496396958842</v>
       </c>
       <c r="AC29">
-        <v>2.5000000000000001E-2</v>
+        <v>25</v>
       </c>
       <c r="AE29">
         <v>4056255.2</v>
@@ -2107,13 +2328,13 @@
     </row>
     <row r="30" spans="2:34" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C30" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="D30" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E30">
         <v>4</v>
@@ -2133,6 +2354,12 @@
       <c r="N30">
         <v>2300</v>
       </c>
+      <c r="S30">
+        <v>2.25</v>
+      </c>
+      <c r="T30">
+        <v>0.15</v>
+      </c>
       <c r="U30">
         <v>2.25</v>
       </c>
@@ -2140,7 +2367,7 @@
         <v>0.15</v>
       </c>
       <c r="AC30">
-        <v>2.5000000000000001E-2</v>
+        <v>25</v>
       </c>
       <c r="AE30">
         <v>4589511.5</v>
@@ -2151,13 +2378,13 @@
     </row>
     <row r="31" spans="2:34" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="C31" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="D31" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E31">
         <v>5</v>
@@ -2177,6 +2404,12 @@
       <c r="N31">
         <v>2300</v>
       </c>
+      <c r="S31">
+        <v>1.2</v>
+      </c>
+      <c r="T31">
+        <v>0.15</v>
+      </c>
       <c r="U31">
         <v>1.2</v>
       </c>
@@ -2190,7 +2423,7 @@
         <v>293.01038835475441</v>
       </c>
       <c r="AC31">
-        <v>2.5000000000000001E-2</v>
+        <v>25</v>
       </c>
       <c r="AE31">
         <v>5129930.9000000004</v>
@@ -2201,13 +2434,13 @@
     </row>
     <row r="32" spans="2:34" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C32" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="D32" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E32">
         <v>6</v>
@@ -2227,6 +2460,12 @@
       <c r="N32">
         <v>2300</v>
       </c>
+      <c r="S32">
+        <v>3.15</v>
+      </c>
+      <c r="T32">
+        <v>0.15</v>
+      </c>
       <c r="U32">
         <v>3.15</v>
       </c>
@@ -2240,7 +2479,7 @@
         <v>2353.9938189586978</v>
       </c>
       <c r="AC32">
-        <v>2.5000000000000001E-2</v>
+        <v>25</v>
       </c>
       <c r="AE32">
         <v>4347129.0999999996</v>
@@ -2251,13 +2490,13 @@
     </row>
     <row r="33" spans="2:39" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C33" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="D33" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E33">
         <v>7</v>
@@ -2277,6 +2516,12 @@
       <c r="N33">
         <v>2300</v>
       </c>
+      <c r="S33">
+        <v>3.6</v>
+      </c>
+      <c r="T33">
+        <v>0.15</v>
+      </c>
       <c r="U33">
         <v>3.6</v>
       </c>
@@ -2290,7 +2535,7 @@
         <v>2349.6763792928391</v>
       </c>
       <c r="AC33">
-        <v>2.5000000000000001E-2</v>
+        <v>25</v>
       </c>
       <c r="AE33">
         <v>4140068.8</v>
@@ -2301,13 +2546,13 @@
     </row>
     <row r="34" spans="2:39" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
+        <v>79</v>
+      </c>
+      <c r="C34" t="s">
         <v>73</v>
       </c>
-      <c r="C34" t="s">
-        <v>67</v>
-      </c>
       <c r="D34" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E34">
         <v>8</v>
@@ -2327,6 +2572,12 @@
       <c r="N34">
         <v>2300</v>
       </c>
+      <c r="S34">
+        <v>4.8</v>
+      </c>
+      <c r="T34">
+        <v>0.15</v>
+      </c>
       <c r="U34">
         <v>4.8</v>
       </c>
@@ -2340,7 +2591,7 @@
         <v>2354.5998481166612</v>
       </c>
       <c r="AC34">
-        <v>2.5000000000000001E-2</v>
+        <v>25</v>
       </c>
       <c r="AE34">
         <v>3850424.2</v>
@@ -2351,13 +2602,13 @@
     </row>
     <row r="35" spans="2:39" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="C35" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="D35" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E35">
         <v>9</v>
@@ -2377,6 +2628,12 @@
       <c r="N35">
         <v>2300</v>
       </c>
+      <c r="S35">
+        <v>4.2</v>
+      </c>
+      <c r="T35">
+        <v>0.15</v>
+      </c>
       <c r="U35">
         <v>4.2</v>
       </c>
@@ -2392,13 +2649,13 @@
     </row>
     <row r="36" spans="2:39" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="C36" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="D36" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E36">
         <v>1</v>
@@ -2422,7 +2679,7 @@
         <v>821</v>
       </c>
       <c r="Q36" t="s">
-        <v>36</v>
+        <v>83</v>
       </c>
       <c r="S36">
         <v>4.2</v>
@@ -2443,7 +2700,7 @@
         <v>2353.5751308215899</v>
       </c>
       <c r="AC36">
-        <v>2.5000000000000001E-2</v>
+        <v>25</v>
       </c>
       <c r="AE36">
         <v>3996936.5</v>
@@ -2454,13 +2711,13 @@
     </row>
     <row r="37" spans="2:39" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C37" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="D37" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E37">
         <v>2</v>
@@ -2484,7 +2741,7 @@
         <v>555</v>
       </c>
       <c r="Q37" t="s">
-        <v>36</v>
+        <v>83</v>
       </c>
       <c r="S37">
         <v>2.25</v>
@@ -2505,7 +2762,7 @@
         <v>1473.4822206123811</v>
       </c>
       <c r="AC37">
-        <v>2.5000000000000001E-2</v>
+        <v>25</v>
       </c>
       <c r="AE37">
         <v>4640377.9000000004</v>
@@ -2523,18 +2780,18 @@
         <v>2297.057543601155</v>
       </c>
       <c r="AM37" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
     </row>
     <row r="38" spans="2:39" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="C38" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="D38" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E38">
         <v>3</v>
@@ -2573,7 +2830,7 @@
         <v>316.06099097493518</v>
       </c>
       <c r="AC38">
-        <v>2.5000000000000001E-2</v>
+        <v>25</v>
       </c>
       <c r="AE38">
         <v>5097601</v>
@@ -2591,18 +2848,18 @@
         <v>2284.6445065762809</v>
       </c>
       <c r="AM38" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
     </row>
     <row r="39" spans="2:39" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="C39" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="D39" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E39">
         <v>4</v>
@@ -2641,7 +2898,7 @@
         <v>321.52978738815011</v>
       </c>
       <c r="AC39">
-        <v>2.5000000000000001E-2</v>
+        <v>25</v>
       </c>
       <c r="AE39">
         <v>4970468.2</v>
@@ -2655,13 +2912,13 @@
     </row>
     <row r="40" spans="2:39" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="C40" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="D40" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E40">
         <v>5</v>
@@ -2700,7 +2957,7 @@
         <v>321.95994581450168</v>
       </c>
       <c r="AC40">
-        <v>2.5000000000000001E-2</v>
+        <v>25</v>
       </c>
       <c r="AE40">
         <v>5091844</v>
@@ -2711,13 +2968,13 @@
     </row>
     <row r="41" spans="2:39" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="C41" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="D41" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E41">
         <v>7</v>
@@ -2741,7 +2998,7 @@
         <v>539</v>
       </c>
       <c r="Q41" t="s">
-        <v>36</v>
+        <v>83</v>
       </c>
       <c r="S41">
         <v>2.25</v>
@@ -2762,7 +3019,7 @@
         <v>1381.2133427804949</v>
       </c>
       <c r="AC41">
-        <v>2.5000000000000001E-2</v>
+        <v>25</v>
       </c>
       <c r="AE41">
         <v>4686458.3</v>
@@ -2773,13 +3030,13 @@
     </row>
     <row r="42" spans="2:39" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
+        <v>90</v>
+      </c>
+      <c r="C42" t="s">
         <v>82</v>
       </c>
-      <c r="C42" t="s">
-        <v>76</v>
-      </c>
       <c r="D42" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E42">
         <v>8</v>
@@ -2803,7 +3060,7 @@
         <v>548</v>
       </c>
       <c r="Q42" t="s">
-        <v>36</v>
+        <v>83</v>
       </c>
       <c r="S42">
         <v>2.25</v>
@@ -2824,7 +3081,7 @@
         <v>1378.574262684311</v>
       </c>
       <c r="AC42">
-        <v>2.5000000000000001E-2</v>
+        <v>25</v>
       </c>
       <c r="AE42">
         <v>4664614.5999999996</v>
@@ -2835,13 +3092,13 @@
     </row>
     <row r="43" spans="2:39" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="C43" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="D43" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E43">
         <v>9</v>
@@ -2865,7 +3122,7 @@
         <v>561</v>
       </c>
       <c r="Q43" t="s">
-        <v>36</v>
+        <v>83</v>
       </c>
       <c r="S43">
         <v>2.25</v>
@@ -2886,7 +3143,7 @@
         <v>1375.7846896123549</v>
       </c>
       <c r="AC43">
-        <v>2.5000000000000001E-2</v>
+        <v>25</v>
       </c>
       <c r="AE43">
         <v>4653102</v>
@@ -2897,13 +3154,13 @@
     </row>
     <row r="44" spans="2:39" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="C44" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="D44" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E44">
         <v>10</v>
@@ -2945,7 +3202,7 @@
         <v>2371.9008162905789</v>
       </c>
       <c r="AC44">
-        <v>2.5000000000000001E-2</v>
+        <v>25</v>
       </c>
       <c r="AE44">
         <v>4331237</v>
@@ -2956,13 +3213,13 @@
     </row>
     <row r="45" spans="2:39" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="C45" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="D45" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E45">
         <v>11</v>
@@ -3004,7 +3261,7 @@
         <v>2370.614220229178</v>
       </c>
       <c r="AC45">
-        <v>2.5000000000000001E-2</v>
+        <v>25</v>
       </c>
       <c r="AE45">
         <v>4366788.8</v>
@@ -3015,13 +3272,13 @@
     </row>
     <row r="46" spans="2:39" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="C46" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="D46" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E46">
         <v>12</v>
@@ -3063,7 +3320,7 @@
         <v>2370.381440353894</v>
       </c>
       <c r="AC46">
-        <v>2.5000000000000001E-2</v>
+        <v>25</v>
       </c>
       <c r="AE46">
         <v>4070656.6</v>
@@ -3074,13 +3331,13 @@
     </row>
     <row r="47" spans="2:39" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="C47" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="D47" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E47">
         <v>13</v>
@@ -3119,14 +3376,1259 @@
         <v>2372.426943327805</v>
       </c>
       <c r="AC47">
-        <v>2.5000000000000001E-2</v>
+        <v>25</v>
       </c>
       <c r="AE47">
         <v>4101739.2</v>
       </c>
       <c r="AF47">
-        <f>AE47/(0.025*AH2)</f>
         <v>1700.461245143907</v>
+      </c>
+    </row>
+    <row r="48" spans="2:39" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>96</v>
+      </c>
+      <c r="C48" t="s">
+        <v>97</v>
+      </c>
+      <c r="D48" t="s">
+        <v>41</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="G48">
+        <v>37</v>
+      </c>
+      <c r="J48">
+        <v>24</v>
+      </c>
+      <c r="K48">
+        <v>170.95</v>
+      </c>
+      <c r="L48">
+        <v>30</v>
+      </c>
+      <c r="M48">
+        <v>0.1</v>
+      </c>
+      <c r="N48">
+        <v>2316</v>
+      </c>
+      <c r="O48" t="s">
+        <v>98</v>
+      </c>
+      <c r="S48">
+        <v>4.2</v>
+      </c>
+      <c r="T48">
+        <v>0.15</v>
+      </c>
+      <c r="U48">
+        <v>4.2</v>
+      </c>
+      <c r="V48">
+        <v>0.15</v>
+      </c>
+      <c r="W48">
+        <v>632.61427340102182</v>
+      </c>
+      <c r="Y48">
+        <v>2144.1953324520978</v>
+      </c>
+      <c r="Z48">
+        <v>2143.31749558193</v>
+      </c>
+      <c r="AC48">
+        <v>20.833333</v>
+      </c>
+      <c r="AE48">
+        <v>3238983</v>
+      </c>
+      <c r="AF48">
+        <v>1611.34530092516</v>
+      </c>
+    </row>
+    <row r="49" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>99</v>
+      </c>
+      <c r="C49" t="s">
+        <v>97</v>
+      </c>
+      <c r="D49" t="s">
+        <v>41</v>
+      </c>
+      <c r="E49">
+        <v>2</v>
+      </c>
+      <c r="G49">
+        <v>42</v>
+      </c>
+      <c r="J49">
+        <v>25.9</v>
+      </c>
+      <c r="K49">
+        <v>171.75</v>
+      </c>
+      <c r="L49">
+        <v>30</v>
+      </c>
+      <c r="M49">
+        <v>0.1</v>
+      </c>
+      <c r="N49">
+        <v>2316</v>
+      </c>
+      <c r="O49" t="s">
+        <v>98</v>
+      </c>
+      <c r="S49">
+        <v>4.2</v>
+      </c>
+      <c r="T49">
+        <v>0.15</v>
+      </c>
+      <c r="U49">
+        <v>4.2</v>
+      </c>
+      <c r="V49">
+        <v>0.15</v>
+      </c>
+      <c r="W49">
+        <v>634.85683079114142</v>
+      </c>
+      <c r="Y49">
+        <v>2186.5078206889029</v>
+      </c>
+      <c r="Z49">
+        <v>2187.733454519685</v>
+      </c>
+      <c r="AC49">
+        <v>20.833333</v>
+      </c>
+      <c r="AE49">
+        <v>3156939.1</v>
+      </c>
+      <c r="AF49">
+        <v>1570.52969530618</v>
+      </c>
+    </row>
+    <row r="50" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
+        <v>100</v>
+      </c>
+      <c r="C50" t="s">
+        <v>97</v>
+      </c>
+      <c r="D50" t="s">
+        <v>41</v>
+      </c>
+      <c r="E50">
+        <v>3</v>
+      </c>
+      <c r="J50">
+        <v>25</v>
+      </c>
+      <c r="K50">
+        <v>171.4</v>
+      </c>
+      <c r="L50">
+        <v>30</v>
+      </c>
+      <c r="M50">
+        <v>0.1</v>
+      </c>
+      <c r="N50">
+        <v>2316</v>
+      </c>
+      <c r="O50" t="s">
+        <v>98</v>
+      </c>
+      <c r="S50">
+        <v>4.2</v>
+      </c>
+      <c r="T50">
+        <v>0.15</v>
+      </c>
+      <c r="U50">
+        <v>4.2</v>
+      </c>
+      <c r="V50">
+        <v>0.15</v>
+      </c>
+      <c r="W50">
+        <v>633.58461882023494</v>
+      </c>
+      <c r="Y50">
+        <v>2197.502496978354</v>
+      </c>
+      <c r="Z50">
+        <v>2197.502496978354</v>
+      </c>
+    </row>
+    <row r="51" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
+        <v>101</v>
+      </c>
+      <c r="C51" t="s">
+        <v>97</v>
+      </c>
+      <c r="D51" t="s">
+        <v>41</v>
+      </c>
+      <c r="E51">
+        <v>4</v>
+      </c>
+      <c r="G51">
+        <v>46</v>
+      </c>
+      <c r="J51">
+        <v>25.1</v>
+      </c>
+      <c r="K51">
+        <v>171.35</v>
+      </c>
+      <c r="L51">
+        <v>30</v>
+      </c>
+      <c r="M51">
+        <v>0.1</v>
+      </c>
+      <c r="N51">
+        <v>2316</v>
+      </c>
+      <c r="O51" t="s">
+        <v>98</v>
+      </c>
+      <c r="S51">
+        <v>4.2</v>
+      </c>
+      <c r="T51">
+        <v>0.15</v>
+      </c>
+      <c r="U51">
+        <v>4.2</v>
+      </c>
+      <c r="V51">
+        <v>0.15</v>
+      </c>
+      <c r="W51">
+        <v>632.05138898594009</v>
+      </c>
+      <c r="Y51">
+        <v>2334.5448620200191</v>
+      </c>
+      <c r="Z51">
+        <v>2334.678236514013</v>
+      </c>
+      <c r="AC51">
+        <v>20.833333</v>
+      </c>
+      <c r="AE51">
+        <v>3070776.2</v>
+      </c>
+      <c r="AF51">
+        <v>1527.66494917164</v>
+      </c>
+    </row>
+    <row r="52" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
+        <v>102</v>
+      </c>
+      <c r="C52" t="s">
+        <v>97</v>
+      </c>
+      <c r="D52" t="s">
+        <v>41</v>
+      </c>
+      <c r="E52">
+        <v>5</v>
+      </c>
+      <c r="G52">
+        <v>51</v>
+      </c>
+      <c r="J52">
+        <v>25.1</v>
+      </c>
+      <c r="K52">
+        <v>171.1</v>
+      </c>
+      <c r="L52">
+        <v>30</v>
+      </c>
+      <c r="M52">
+        <v>0.1</v>
+      </c>
+      <c r="N52">
+        <v>2316</v>
+      </c>
+      <c r="O52" t="s">
+        <v>98</v>
+      </c>
+      <c r="S52">
+        <v>4.2</v>
+      </c>
+      <c r="T52">
+        <v>0.15</v>
+      </c>
+      <c r="U52">
+        <v>4.2</v>
+      </c>
+      <c r="V52">
+        <v>0.15</v>
+      </c>
+      <c r="W52">
+        <v>632.08729778326051</v>
+      </c>
+      <c r="Y52">
+        <v>2335.2943411657102</v>
+      </c>
+      <c r="Z52">
+        <v>2335.427685555791</v>
+      </c>
+      <c r="AC52">
+        <v>20.833333</v>
+      </c>
+      <c r="AE52">
+        <v>3152471.5</v>
+      </c>
+      <c r="AF52">
+        <v>1568.3071315365</v>
+      </c>
+    </row>
+    <row r="53" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>103</v>
+      </c>
+      <c r="C53" t="s">
+        <v>97</v>
+      </c>
+      <c r="D53" t="s">
+        <v>41</v>
+      </c>
+      <c r="E53">
+        <v>7</v>
+      </c>
+      <c r="J53">
+        <v>25.2</v>
+      </c>
+      <c r="K53">
+        <v>170.85</v>
+      </c>
+      <c r="L53">
+        <v>30</v>
+      </c>
+      <c r="M53">
+        <v>0.1</v>
+      </c>
+      <c r="N53">
+        <v>2316</v>
+      </c>
+      <c r="O53" t="s">
+        <v>98</v>
+      </c>
+      <c r="S53">
+        <v>2.25</v>
+      </c>
+      <c r="T53">
+        <v>0.15</v>
+      </c>
+      <c r="U53">
+        <v>2.25</v>
+      </c>
+      <c r="V53">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="54" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
+        <v>104</v>
+      </c>
+      <c r="C54" t="s">
+        <v>97</v>
+      </c>
+      <c r="D54" t="s">
+        <v>41</v>
+      </c>
+      <c r="E54">
+        <v>8</v>
+      </c>
+      <c r="G54">
+        <v>54</v>
+      </c>
+      <c r="J54">
+        <v>25.2</v>
+      </c>
+      <c r="K54">
+        <v>170.35</v>
+      </c>
+      <c r="L54">
+        <v>30</v>
+      </c>
+      <c r="M54">
+        <v>0.1</v>
+      </c>
+      <c r="N54">
+        <v>2316</v>
+      </c>
+      <c r="O54" t="s">
+        <v>98</v>
+      </c>
+      <c r="S54">
+        <v>2.25</v>
+      </c>
+      <c r="T54">
+        <v>0.15</v>
+      </c>
+      <c r="U54">
+        <v>2.25</v>
+      </c>
+      <c r="V54">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="55" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B55" t="s">
+        <v>105</v>
+      </c>
+      <c r="C55" t="s">
+        <v>97</v>
+      </c>
+      <c r="D55" t="s">
+        <v>41</v>
+      </c>
+      <c r="E55">
+        <v>9</v>
+      </c>
+      <c r="G55">
+        <v>55</v>
+      </c>
+      <c r="J55">
+        <v>25.2</v>
+      </c>
+      <c r="K55">
+        <v>170.2</v>
+      </c>
+      <c r="L55">
+        <v>30</v>
+      </c>
+      <c r="M55">
+        <v>0.1</v>
+      </c>
+      <c r="N55">
+        <v>2316</v>
+      </c>
+      <c r="O55" t="s">
+        <v>98</v>
+      </c>
+      <c r="S55">
+        <v>2.25</v>
+      </c>
+      <c r="T55">
+        <v>0.15</v>
+      </c>
+      <c r="U55">
+        <v>2.25</v>
+      </c>
+      <c r="V55">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="56" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B56" t="s">
+        <v>106</v>
+      </c>
+      <c r="C56" t="s">
+        <v>107</v>
+      </c>
+      <c r="D56" t="s">
+        <v>41</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+      <c r="G56">
+        <v>59</v>
+      </c>
+      <c r="J56">
+        <v>24.7</v>
+      </c>
+      <c r="K56">
+        <v>170.05</v>
+      </c>
+      <c r="L56">
+        <v>30</v>
+      </c>
+      <c r="M56">
+        <v>0.1</v>
+      </c>
+      <c r="N56">
+        <v>2280</v>
+      </c>
+      <c r="O56" t="s">
+        <v>98</v>
+      </c>
+      <c r="S56">
+        <v>4.2</v>
+      </c>
+      <c r="T56">
+        <v>0.15</v>
+      </c>
+      <c r="U56">
+        <v>4.2</v>
+      </c>
+      <c r="V56">
+        <v>0.15</v>
+      </c>
+      <c r="W56">
+        <v>631.54115521632514</v>
+      </c>
+      <c r="Y56">
+        <v>2295.0304980356809</v>
+      </c>
+    </row>
+    <row r="57" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B57" t="s">
+        <v>108</v>
+      </c>
+      <c r="C57" t="s">
+        <v>107</v>
+      </c>
+      <c r="D57" t="s">
+        <v>41</v>
+      </c>
+      <c r="E57">
+        <v>2</v>
+      </c>
+      <c r="G57">
+        <v>61</v>
+      </c>
+      <c r="J57">
+        <v>24.7</v>
+      </c>
+      <c r="K57">
+        <v>169.75</v>
+      </c>
+      <c r="L57">
+        <v>30</v>
+      </c>
+      <c r="M57">
+        <v>0.1</v>
+      </c>
+      <c r="N57">
+        <v>2280</v>
+      </c>
+      <c r="O57" t="s">
+        <v>98</v>
+      </c>
+      <c r="S57">
+        <v>4.2</v>
+      </c>
+      <c r="T57">
+        <v>0.15</v>
+      </c>
+      <c r="U57">
+        <v>4.2</v>
+      </c>
+      <c r="V57">
+        <v>0.15</v>
+      </c>
+      <c r="W57">
+        <v>631.66140214666757</v>
+      </c>
+      <c r="Y57">
+        <v>2301.8384531650458</v>
+      </c>
+    </row>
+    <row r="58" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B58" t="s">
+        <v>109</v>
+      </c>
+      <c r="C58" t="s">
+        <v>107</v>
+      </c>
+      <c r="D58" t="s">
+        <v>41</v>
+      </c>
+      <c r="E58">
+        <v>3</v>
+      </c>
+      <c r="G58">
+        <v>62</v>
+      </c>
+      <c r="J58">
+        <v>25.2</v>
+      </c>
+      <c r="K58">
+        <v>169.9</v>
+      </c>
+      <c r="L58">
+        <v>30</v>
+      </c>
+      <c r="M58">
+        <v>0.1</v>
+      </c>
+      <c r="N58">
+        <v>2280</v>
+      </c>
+      <c r="O58" t="s">
+        <v>98</v>
+      </c>
+      <c r="S58">
+        <v>4.2</v>
+      </c>
+      <c r="T58">
+        <v>0.15</v>
+      </c>
+      <c r="U58">
+        <v>4.2</v>
+      </c>
+      <c r="V58">
+        <v>0.15</v>
+      </c>
+      <c r="W58">
+        <v>632.01025337810415</v>
+      </c>
+      <c r="Y58">
+        <v>2302.0758407055969</v>
+      </c>
+    </row>
+    <row r="59" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B59" t="s">
+        <v>110</v>
+      </c>
+      <c r="C59" t="s">
+        <v>107</v>
+      </c>
+      <c r="D59" t="s">
+        <v>41</v>
+      </c>
+      <c r="E59">
+        <v>4</v>
+      </c>
+      <c r="G59">
+        <v>63</v>
+      </c>
+      <c r="J59">
+        <v>25.2</v>
+      </c>
+      <c r="K59">
+        <v>169.75</v>
+      </c>
+      <c r="L59">
+        <v>30</v>
+      </c>
+      <c r="M59">
+        <v>0.1</v>
+      </c>
+      <c r="N59">
+        <v>2280</v>
+      </c>
+      <c r="O59" t="s">
+        <v>98</v>
+      </c>
+      <c r="S59">
+        <v>4.2</v>
+      </c>
+      <c r="T59">
+        <v>0.15</v>
+      </c>
+      <c r="U59">
+        <v>4.2</v>
+      </c>
+      <c r="V59">
+        <v>0.15</v>
+      </c>
+      <c r="W59">
+        <v>631.95860521483712</v>
+      </c>
+      <c r="Y59">
+        <v>2301.0539740141749</v>
+      </c>
+    </row>
+    <row r="60" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B60" t="s">
+        <v>111</v>
+      </c>
+      <c r="C60" t="s">
+        <v>107</v>
+      </c>
+      <c r="D60" t="s">
+        <v>41</v>
+      </c>
+      <c r="E60">
+        <v>5</v>
+      </c>
+      <c r="G60">
+        <v>64</v>
+      </c>
+      <c r="J60">
+        <v>25.1</v>
+      </c>
+      <c r="K60">
+        <v>169.75</v>
+      </c>
+      <c r="L60">
+        <v>30</v>
+      </c>
+      <c r="M60">
+        <v>0.1</v>
+      </c>
+      <c r="N60">
+        <v>2280</v>
+      </c>
+      <c r="O60" t="s">
+        <v>98</v>
+      </c>
+      <c r="S60">
+        <v>4.2</v>
+      </c>
+      <c r="T60">
+        <v>0.15</v>
+      </c>
+      <c r="U60">
+        <v>4.2</v>
+      </c>
+      <c r="V60">
+        <v>0.15</v>
+      </c>
+      <c r="W60">
+        <v>631.95773256193331</v>
+      </c>
+      <c r="Y60">
+        <v>2299.9137965893578</v>
+      </c>
+    </row>
+    <row r="61" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B61" t="s">
+        <v>112</v>
+      </c>
+      <c r="C61" t="s">
+        <v>107</v>
+      </c>
+      <c r="D61" t="s">
+        <v>41</v>
+      </c>
+      <c r="E61">
+        <v>6</v>
+      </c>
+      <c r="G61">
+        <v>65</v>
+      </c>
+      <c r="J61">
+        <v>25.1</v>
+      </c>
+      <c r="K61">
+        <v>169.65</v>
+      </c>
+      <c r="L61">
+        <v>30</v>
+      </c>
+      <c r="M61">
+        <v>0.1</v>
+      </c>
+      <c r="N61">
+        <v>2280</v>
+      </c>
+      <c r="O61" t="s">
+        <v>98</v>
+      </c>
+      <c r="S61">
+        <v>4.2</v>
+      </c>
+      <c r="T61">
+        <v>0.15</v>
+      </c>
+      <c r="U61">
+        <v>4.2</v>
+      </c>
+      <c r="V61">
+        <v>0.15</v>
+      </c>
+      <c r="W61">
+        <v>631.89276175656516</v>
+      </c>
+      <c r="Y61">
+        <v>2297.0464505237592</v>
+      </c>
+    </row>
+    <row r="62" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B62" t="s">
+        <v>113</v>
+      </c>
+      <c r="C62" t="s">
+        <v>107</v>
+      </c>
+      <c r="D62" t="s">
+        <v>41</v>
+      </c>
+      <c r="E62">
+        <v>7</v>
+      </c>
+      <c r="G62">
+        <v>66</v>
+      </c>
+      <c r="J62">
+        <v>25.1</v>
+      </c>
+      <c r="K62">
+        <v>169.5</v>
+      </c>
+      <c r="L62">
+        <v>30</v>
+      </c>
+      <c r="M62">
+        <v>0.1</v>
+      </c>
+      <c r="N62">
+        <v>2280</v>
+      </c>
+      <c r="O62" t="s">
+        <v>98</v>
+      </c>
+      <c r="S62">
+        <v>4.2</v>
+      </c>
+      <c r="T62">
+        <v>0.15</v>
+      </c>
+      <c r="U62">
+        <v>4.2</v>
+      </c>
+      <c r="V62">
+        <v>0.15</v>
+      </c>
+      <c r="W62">
+        <v>631.9037751258827</v>
+      </c>
+      <c r="Y62">
+        <v>2300.4511879227612</v>
+      </c>
+    </row>
+    <row r="63" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B63" t="s">
+        <v>114</v>
+      </c>
+      <c r="C63" t="s">
+        <v>107</v>
+      </c>
+      <c r="D63" t="s">
+        <v>41</v>
+      </c>
+      <c r="E63">
+        <v>8</v>
+      </c>
+      <c r="G63">
+        <v>67</v>
+      </c>
+      <c r="J63">
+        <v>25.1</v>
+      </c>
+      <c r="K63">
+        <v>169.55</v>
+      </c>
+      <c r="L63">
+        <v>30</v>
+      </c>
+      <c r="M63">
+        <v>0.1</v>
+      </c>
+      <c r="N63">
+        <v>2280</v>
+      </c>
+      <c r="O63" t="s">
+        <v>98</v>
+      </c>
+      <c r="S63">
+        <v>4.2</v>
+      </c>
+      <c r="T63">
+        <v>0.15</v>
+      </c>
+      <c r="U63">
+        <v>4.2</v>
+      </c>
+      <c r="V63">
+        <v>0.15</v>
+      </c>
+      <c r="W63">
+        <v>631.90650742590651</v>
+      </c>
+      <c r="Y63">
+        <v>2299.3528756602191</v>
+      </c>
+    </row>
+    <row r="64" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B64" t="s">
+        <v>115</v>
+      </c>
+      <c r="C64" t="s">
+        <v>116</v>
+      </c>
+      <c r="D64" t="s">
+        <v>41</v>
+      </c>
+      <c r="E64">
+        <v>1</v>
+      </c>
+      <c r="G64">
+        <v>72</v>
+      </c>
+      <c r="J64">
+        <v>25.1</v>
+      </c>
+      <c r="K64">
+        <v>167.75</v>
+      </c>
+      <c r="L64">
+        <v>30</v>
+      </c>
+      <c r="M64">
+        <v>0.1</v>
+      </c>
+      <c r="N64">
+        <v>2265</v>
+      </c>
+      <c r="O64" t="s">
+        <v>98</v>
+      </c>
+      <c r="S64">
+        <v>4.2</v>
+      </c>
+      <c r="T64">
+        <v>0.15</v>
+      </c>
+      <c r="U64">
+        <v>4.2</v>
+      </c>
+      <c r="V64">
+        <v>0.15</v>
+      </c>
+      <c r="W64">
+        <v>631.86939453180707</v>
+      </c>
+      <c r="Y64">
+        <v>2297.1001762973542</v>
+      </c>
+    </row>
+    <row r="65" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="B65" t="s">
+        <v>117</v>
+      </c>
+      <c r="C65" t="s">
+        <v>116</v>
+      </c>
+      <c r="D65" t="s">
+        <v>41</v>
+      </c>
+      <c r="E65">
+        <v>2</v>
+      </c>
+      <c r="G65">
+        <v>74</v>
+      </c>
+      <c r="J65">
+        <v>25.1</v>
+      </c>
+      <c r="K65">
+        <v>167.85</v>
+      </c>
+      <c r="L65">
+        <v>30</v>
+      </c>
+      <c r="M65">
+        <v>0.1</v>
+      </c>
+      <c r="N65">
+        <v>2265</v>
+      </c>
+      <c r="O65" t="s">
+        <v>98</v>
+      </c>
+      <c r="S65">
+        <v>4.2</v>
+      </c>
+      <c r="T65">
+        <v>0.15</v>
+      </c>
+      <c r="U65">
+        <v>4.2</v>
+      </c>
+      <c r="V65">
+        <v>0.15</v>
+      </c>
+      <c r="W65">
+        <v>631.84489790527266</v>
+      </c>
+      <c r="Y65">
+        <v>2297.322107195424</v>
+      </c>
+    </row>
+    <row r="66" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="B66" t="s">
+        <v>118</v>
+      </c>
+      <c r="C66" t="s">
+        <v>116</v>
+      </c>
+      <c r="D66" t="s">
+        <v>41</v>
+      </c>
+      <c r="E66">
+        <v>3</v>
+      </c>
+      <c r="G66">
+        <v>75</v>
+      </c>
+      <c r="J66">
+        <v>25.1</v>
+      </c>
+      <c r="K66">
+        <v>167.55</v>
+      </c>
+      <c r="L66">
+        <v>30</v>
+      </c>
+      <c r="M66">
+        <v>0.1</v>
+      </c>
+      <c r="N66">
+        <v>2265</v>
+      </c>
+      <c r="O66" t="s">
+        <v>98</v>
+      </c>
+      <c r="S66">
+        <v>4.2</v>
+      </c>
+      <c r="T66">
+        <v>0.15</v>
+      </c>
+      <c r="U66">
+        <v>4.2</v>
+      </c>
+      <c r="V66">
+        <v>0.15</v>
+      </c>
+      <c r="W66">
+        <v>631.85341623166232</v>
+      </c>
+      <c r="Y66">
+        <v>2298.1080543003659</v>
+      </c>
+    </row>
+    <row r="67" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="B67" t="s">
+        <v>119</v>
+      </c>
+      <c r="C67" t="s">
+        <v>116</v>
+      </c>
+      <c r="D67" t="s">
+        <v>41</v>
+      </c>
+      <c r="E67">
+        <v>4</v>
+      </c>
+      <c r="G67">
+        <v>77</v>
+      </c>
+      <c r="J67">
+        <v>25.2</v>
+      </c>
+      <c r="K67">
+        <v>167.55</v>
+      </c>
+      <c r="L67">
+        <v>30</v>
+      </c>
+      <c r="M67">
+        <v>0.1</v>
+      </c>
+      <c r="N67">
+        <v>2265</v>
+      </c>
+      <c r="O67" t="s">
+        <v>98</v>
+      </c>
+      <c r="S67">
+        <v>4.2</v>
+      </c>
+      <c r="T67">
+        <v>0.15</v>
+      </c>
+      <c r="U67">
+        <v>4.2</v>
+      </c>
+      <c r="V67">
+        <v>0.15</v>
+      </c>
+      <c r="W67">
+        <v>631.93929532282596</v>
+      </c>
+      <c r="Y67">
+        <v>2298.9700802401212</v>
+      </c>
+    </row>
+    <row r="68" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="B68" t="s">
+        <v>120</v>
+      </c>
+      <c r="C68" t="s">
+        <v>116</v>
+      </c>
+      <c r="D68" t="s">
+        <v>41</v>
+      </c>
+      <c r="E68">
+        <v>5</v>
+      </c>
+      <c r="G68">
+        <v>79</v>
+      </c>
+      <c r="J68">
+        <v>25.2</v>
+      </c>
+      <c r="K68">
+        <v>167.4</v>
+      </c>
+      <c r="L68">
+        <v>30</v>
+      </c>
+      <c r="M68">
+        <v>0.1</v>
+      </c>
+      <c r="N68">
+        <v>2265</v>
+      </c>
+      <c r="O68" t="s">
+        <v>98</v>
+      </c>
+      <c r="S68">
+        <v>4.2</v>
+      </c>
+      <c r="T68">
+        <v>0.15</v>
+      </c>
+      <c r="U68">
+        <v>4.2</v>
+      </c>
+      <c r="V68">
+        <v>0.15</v>
+      </c>
+      <c r="W68">
+        <v>632.0255973355537</v>
+      </c>
+      <c r="Y68">
+        <v>2303.2723704869331</v>
+      </c>
+    </row>
+    <row r="69" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="B69" t="s">
+        <v>121</v>
+      </c>
+      <c r="C69" t="s">
+        <v>116</v>
+      </c>
+      <c r="D69" t="s">
+        <v>41</v>
+      </c>
+      <c r="E69">
+        <v>6</v>
+      </c>
+      <c r="G69">
+        <v>80</v>
+      </c>
+      <c r="J69">
+        <v>25.1</v>
+      </c>
+      <c r="K69">
+        <v>166.65</v>
+      </c>
+      <c r="L69">
+        <v>30</v>
+      </c>
+      <c r="M69">
+        <v>0.1</v>
+      </c>
+      <c r="N69">
+        <v>2265</v>
+      </c>
+      <c r="O69" t="s">
+        <v>98</v>
+      </c>
+      <c r="S69">
+        <v>4.2</v>
+      </c>
+      <c r="T69">
+        <v>0.15</v>
+      </c>
+      <c r="U69">
+        <v>4.2</v>
+      </c>
+      <c r="V69">
+        <v>0.15</v>
+      </c>
+      <c r="W69">
+        <v>631.91351123089294</v>
+      </c>
+      <c r="Y69">
+        <v>2309.3362065417741</v>
+      </c>
+    </row>
+    <row r="70" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="B70" t="s">
+        <v>122</v>
+      </c>
+      <c r="C70" t="s">
+        <v>116</v>
+      </c>
+      <c r="D70" t="s">
+        <v>41</v>
+      </c>
+      <c r="E70">
+        <v>7</v>
+      </c>
+      <c r="G70">
+        <v>81</v>
+      </c>
+      <c r="J70">
+        <v>25.2</v>
+      </c>
+      <c r="K70">
+        <v>166.35</v>
+      </c>
+      <c r="L70">
+        <v>30</v>
+      </c>
+      <c r="M70">
+        <v>0.1</v>
+      </c>
+      <c r="N70">
+        <v>2265</v>
+      </c>
+      <c r="O70" t="s">
+        <v>98</v>
+      </c>
+      <c r="S70">
+        <v>4.2</v>
+      </c>
+      <c r="T70">
+        <v>0.15</v>
+      </c>
+      <c r="U70">
+        <v>4.2</v>
+      </c>
+      <c r="V70">
+        <v>0.15</v>
+      </c>
+      <c r="W70">
+        <v>632.0035126698524</v>
+      </c>
+      <c r="Y70">
+        <v>2298.9867016215999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>